<commit_message>
Monday - 18/11/2024 - 17:20
</commit_message>
<xml_diff>
--- a/Rating .xlsx
+++ b/Rating .xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Discovery Content\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Discovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A86387-3F9B-40FB-930F-B5DF5B506359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FD415C-9752-4AA9-8A27-467F23D71FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -574,7 +574,7 @@
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -670,6 +670,12 @@
         <v>14</v>
       </c>
       <c r="D12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>